<commit_message>
ETF &  Template Update
</commit_message>
<xml_diff>
--- a/Analysis-Owned_ETF/AMLP - Alerian MLP ETF/data/amlp_data.xlsx
+++ b/Analysis-Owned_ETF/AMLP - Alerian MLP ETF/data/amlp_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10119"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D893891B-7DDC-6F4C-9865-2159B1C59109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909320DE-DF60-8C48-A663-E9776AE2DA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>dividend</t>
   </si>
@@ -37,9 +37,6 @@
     <t>ex_date</t>
   </si>
   <si>
-    <t>year</t>
-  </si>
-  <si>
     <t>ticker</t>
   </si>
   <si>
@@ -131,16 +128,38 @@
   </si>
   <si>
     <t>Cheniere Energy Partners LP</t>
+  </si>
+  <si>
+    <t>multiplier</t>
+  </si>
+  <si>
+    <t>etf_d</t>
+  </si>
+  <si>
+    <t>etf_v</t>
+  </si>
+  <si>
+    <t>etf_y</t>
+  </si>
+  <si>
+    <t>AVE</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>YOC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="mm\/dd\/yyyy"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -180,7 +199,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -188,19 +207,43 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="15">
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -279,11 +322,16 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="mm\/dd\/yyyy"/>
@@ -310,35 +358,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E60671D7-5657-EB4E-90C2-457CCC87C042}" name="Table2" displayName="Table2" ref="A1:C58" totalsRowShown="0" dataDxfId="9">
-  <autoFilter ref="A1:C58" xr:uid="{E60671D7-5657-EB4E-90C2-457CCC87C042}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E60671D7-5657-EB4E-90C2-457CCC87C042}" name="Table2" displayName="Table2" ref="A1:B58" totalsRowShown="0" dataDxfId="14">
+  <autoFilter ref="A1:B58" xr:uid="{E60671D7-5657-EB4E-90C2-457CCC87C042}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B58">
     <sortCondition descending="1" ref="B1:B58"/>
   </sortState>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D7F0A743-B072-484A-B9F8-94695E6993A5}" name="dividend" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{852C8703-7752-E64B-B68C-918F29940680}" name="ex_date" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{ECFDD89A-E4B5-EE40-B8E8-68CF5347A404}" name="year" dataDxfId="6">
-      <calculatedColumnFormula>YEAR(Table2[[#This Row],[ex_date]])</calculatedColumnFormula>
-    </tableColumn>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{D7F0A743-B072-484A-B9F8-94695E6993A5}" name="dividend" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{852C8703-7752-E64B-B68C-918F29940680}" name="ex_date" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0FFF5ED-F252-164C-80A2-73558FC91298}" name="Table1" displayName="Table1" ref="A1:G14" totalsRowCount="1">
-  <autoFilter ref="A1:G13" xr:uid="{B0FFF5ED-F252-164C-80A2-73558FC91298}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0FFF5ED-F252-164C-80A2-73558FC91298}" name="Table1" displayName="Table1" ref="A1:K14" totalsRowCount="1">
+  <autoFilter ref="A1:K13" xr:uid="{B0FFF5ED-F252-164C-80A2-73558FC91298}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{71218243-3960-834F-ACFA-5D5DFCD6DE4F}" name="ticker"/>
     <tableColumn id="2" xr3:uid="{214E5B32-48DF-2241-9EC0-352D2233E039}" name="name"/>
-    <tableColumn id="3" xr3:uid="{92F99026-3D1F-2D48-8119-83093E9C9339}" name="weight" dataDxfId="5" totalsRowDxfId="3" dataCellStyle="Percent" totalsRowCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{92F99026-3D1F-2D48-8119-83093E9C9339}" name="weight" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="6" dataCellStyle="Percent" totalsRowCellStyle="Percent"/>
     <tableColumn id="4" xr3:uid="{FECE75CF-0FFF-1943-A783-CDFCF9958F11}" name="date"/>
-    <tableColumn id="5" xr3:uid="{CB6060C8-3982-7E4D-A336-8AD5450D3A84}" name="fwd_div" totalsRowFunction="sum" totalsRowDxfId="2" dataCellStyle="Currency" totalsRowCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{20D51FEF-C1AD-4545-94C7-6196A1E8FA83}" name="price" totalsRowFunction="sum" totalsRowDxfId="1" dataCellStyle="Currency" totalsRowCellStyle="Currency"/>
-    <tableColumn id="7" xr3:uid="{9837AB2E-8D85-BC43-9032-FC53D6CC8C02}" name="yield" totalsRowFunction="custom" dataDxfId="4" totalsRowDxfId="0" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+    <tableColumn id="5" xr3:uid="{CB6060C8-3982-7E4D-A336-8AD5450D3A84}" name="fwd_div" totalsRowFunction="sum" totalsRowDxfId="5" dataCellStyle="Currency" totalsRowCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{20D51FEF-C1AD-4545-94C7-6196A1E8FA83}" name="price" totalsRowFunction="sum" totalsRowDxfId="4" dataCellStyle="Currency" totalsRowCellStyle="Currency"/>
+    <tableColumn id="7" xr3:uid="{9837AB2E-8D85-BC43-9032-FC53D6CC8C02}" name="yield" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="3" dataCellStyle="Percent" totalsRowCellStyle="Percent">
       <calculatedColumnFormula>Table1[[#This Row],[fwd_div]]/Table1[[#This Row],[price]]</calculatedColumnFormula>
       <totalsRowFormula>Table1[[#Totals],[fwd_div]]/Table1[[#Totals],[price]]</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{17A8FDA1-C843-1D4E-AB59-BF3DDA17ED59}" name="multiplier" totalsRowFunction="sum"/>
+    <tableColumn id="9" xr3:uid="{3A8E334A-2061-6E4D-9B76-E87B601268C9}" name="etf_d" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="1">
+      <calculatedColumnFormula>Table1[[#This Row],[fwd_div]]*Table1[[#This Row],[multiplier]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{2FB80D51-5514-2144-8005-A5F3F5156F11}" name="etf_v" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[multiplier]]*Table1[[#This Row],[price]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{5BC32981-A8D4-C94E-9A90-B3590DA9AB31}" name="etf_y" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="2" dataCellStyle="Percent" totalsRowCellStyle="Percent">
+      <calculatedColumnFormula>Table1[[#This Row],[etf_d]]/Table1[[#This Row],[etf_v]]</calculatedColumnFormula>
+      <totalsRowFormula>Table1[[#Totals],[etf_d]]/Table1[[#Totals],[etf_v]]</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -667,707 +723,476 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DAA334-DBD4-AC45-8A6D-F6AA56E5C671}">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0.95</v>
       </c>
       <c r="B2" s="2">
         <v>45609</v>
       </c>
-      <c r="C2" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0.94</v>
       </c>
       <c r="B3" s="2">
         <v>45512</v>
       </c>
-      <c r="C3" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>0.94</v>
       </c>
       <c r="B4" s="2">
         <v>45421</v>
       </c>
-      <c r="C4" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>0.88</v>
       </c>
       <c r="B5" s="2">
         <v>45330</v>
       </c>
-      <c r="C5" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>0.88</v>
       </c>
       <c r="B6" s="2">
         <v>45239</v>
       </c>
-      <c r="C6" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>0.83</v>
       </c>
       <c r="B7" s="2">
         <v>45148</v>
       </c>
-      <c r="C7" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>0.86</v>
       </c>
       <c r="B8" s="2">
         <v>45057</v>
       </c>
-      <c r="C8" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>0.77</v>
       </c>
       <c r="B9" s="2">
         <v>44966</v>
       </c>
-      <c r="C9" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>0.75</v>
       </c>
       <c r="B10" s="2">
         <v>44874</v>
       </c>
-      <c r="C10" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>0.74</v>
       </c>
       <c r="B11" s="2">
         <v>44784</v>
       </c>
-      <c r="C11" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>0.73</v>
       </c>
       <c r="B12" s="2">
         <v>44693</v>
       </c>
-      <c r="C12" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>0.71</v>
       </c>
       <c r="B13" s="2">
         <v>44602</v>
       </c>
-      <c r="C13" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>0.76</v>
       </c>
       <c r="B14" s="2">
         <v>44510</v>
       </c>
-      <c r="C14" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>0.68</v>
       </c>
       <c r="B15" s="2">
         <v>44420</v>
       </c>
-      <c r="C15" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>0.68</v>
       </c>
       <c r="B16" s="2">
         <v>44329</v>
       </c>
-      <c r="C16" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>0.68</v>
       </c>
       <c r="B17" s="2">
         <v>44238</v>
       </c>
-      <c r="C17" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>0.71</v>
       </c>
       <c r="B18" s="2">
         <v>44147</v>
       </c>
-      <c r="C18" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>0.75</v>
       </c>
       <c r="B19" s="2">
         <v>44056</v>
       </c>
-      <c r="C19" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>0.15</v>
       </c>
       <c r="B20" s="2">
         <v>43958</v>
       </c>
-      <c r="C20" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>0.19</v>
       </c>
       <c r="B21" s="2">
         <v>43874</v>
       </c>
-      <c r="C21" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>0.19500000000000001</v>
       </c>
       <c r="B22" s="2">
         <v>43783</v>
       </c>
-      <c r="C22" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>0.19</v>
       </c>
       <c r="B23" s="2">
         <v>43685</v>
       </c>
-      <c r="C23" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>0.19500000000000001</v>
       </c>
       <c r="B24" s="2">
         <v>43594</v>
       </c>
-      <c r="C24" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>0.19500000000000001</v>
       </c>
       <c r="B25" s="2">
         <v>43510</v>
       </c>
-      <c r="C25" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>0.1913</v>
       </c>
       <c r="B26" s="2">
         <v>43412</v>
       </c>
-      <c r="C26" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>0.20660000000000001</v>
       </c>
       <c r="B27" s="2">
         <v>43321</v>
       </c>
-      <c r="C27" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>0.20660000000000001</v>
       </c>
       <c r="B28" s="2">
         <v>43230</v>
       </c>
-      <c r="C28" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>0.20660000000000001</v>
       </c>
       <c r="B29" s="2">
         <v>43139</v>
       </c>
-      <c r="C29" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>0.20519999999999999</v>
       </c>
       <c r="B30" s="2">
         <v>43048</v>
       </c>
-      <c r="C30" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>0.215</v>
       </c>
       <c r="B31" s="2">
         <v>42956</v>
       </c>
-      <c r="C31" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>0.215</v>
       </c>
       <c r="B32" s="2">
         <v>42865</v>
       </c>
-      <c r="C32" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>0.22500000000000001</v>
       </c>
       <c r="B33" s="2">
         <v>42774</v>
       </c>
-      <c r="C33" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>0.24</v>
       </c>
       <c r="B34" s="2">
         <v>42683</v>
       </c>
-      <c r="C34" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>0.24</v>
       </c>
       <c r="B35" s="2">
         <v>42592</v>
       </c>
-      <c r="C35" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>0.24</v>
       </c>
       <c r="B36" s="2">
         <v>42501</v>
       </c>
-      <c r="C36" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>0.29899999999999999</v>
       </c>
       <c r="B37" s="2">
         <v>42410</v>
       </c>
-      <c r="C37" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>0.29899999999999999</v>
       </c>
       <c r="B38" s="2">
         <v>42318</v>
       </c>
-      <c r="C38" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>0.29899999999999999</v>
       </c>
       <c r="B39" s="2">
         <v>42228</v>
       </c>
-      <c r="C39" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>0.29549999999999998</v>
       </c>
       <c r="B40" s="2">
         <v>42137</v>
       </c>
-      <c r="C40" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>0.29249999999999998</v>
       </c>
       <c r="B41" s="2">
         <v>42046</v>
       </c>
-      <c r="C41" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>0.28899999999999998</v>
       </c>
       <c r="B42" s="2">
         <v>41949</v>
       </c>
-      <c r="C42" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>0.28399999999999997</v>
       </c>
       <c r="B43" s="2">
         <v>41857</v>
       </c>
-      <c r="C43" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>0.27900000000000003</v>
       </c>
       <c r="B44" s="2">
         <v>41765</v>
       </c>
-      <c r="C44" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>0.27800000000000002</v>
       </c>
       <c r="B45" s="2">
         <v>41676</v>
       </c>
-      <c r="C45" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>0.27400000000000002</v>
       </c>
       <c r="B46" s="2">
         <v>41585</v>
       </c>
-      <c r="C46" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>0.26900000000000002</v>
       </c>
       <c r="B47" s="2">
         <v>41493</v>
       </c>
-      <c r="C47" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>0.26400000000000001</v>
       </c>
       <c r="B48" s="2">
         <v>41401</v>
       </c>
-      <c r="C48" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>0.26100000000000001</v>
       </c>
       <c r="B49" s="2">
         <v>41312</v>
       </c>
-      <c r="C49" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>0.25600000000000001</v>
       </c>
       <c r="B50" s="2">
         <v>41220</v>
       </c>
-      <c r="C50" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>0.252</v>
       </c>
       <c r="B51" s="2">
         <v>41128</v>
       </c>
-      <c r="C51" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>0.245</v>
       </c>
       <c r="B52" s="2">
         <v>41036</v>
       </c>
-      <c r="C52" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>0.24296699999999999</v>
       </c>
       <c r="B53" s="2">
         <v>40946</v>
       </c>
-      <c r="C53" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>0.25775199999999998</v>
       </c>
       <c r="B54" s="2">
         <v>40854</v>
       </c>
-      <c r="C54" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>0.252558</v>
       </c>
       <c r="B55" s="2">
         <v>40760</v>
       </c>
-      <c r="C55" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>0.24582999999999999</v>
       </c>
       <c r="B56" s="2">
         <v>40669</v>
       </c>
-      <c r="C56" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>0.24324299999999999</v>
       </c>
       <c r="B57" s="2">
         <v>40581</v>
       </c>
-      <c r="C57" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>0.24793999999999999</v>
       </c>
       <c r="B58" s="2">
         <v>40487</v>
-      </c>
-      <c r="C58" s="3">
-        <f>YEAR(Table2[[#This Row],[ex_date]])</f>
-        <v>2010</v>
       </c>
     </row>
   </sheetData>
@@ -1380,10 +1205,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58DFDF0F-3FC8-CA41-9455-586EC459F8F6}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1391,330 +1216,568 @@
     <col min="2" max="2" width="46.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
       <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="5">
+        <v>27</v>
+      </c>
+      <c r="C2" s="4">
         <v>0.13339999999999999</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>45691</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>1.52</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>19.8</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <f>Table1[[#This Row],[fwd_div]]/Table1[[#This Row],[price]]</f>
         <v>7.6767676767676762E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <f>Table1[[#This Row],[weight]]*100</f>
+        <v>13.34</v>
+      </c>
+      <c r="I2" s="6">
+        <f>Table1[[#This Row],[fwd_div]]*Table1[[#This Row],[multiplier]]</f>
+        <v>20.276800000000001</v>
+      </c>
+      <c r="J2" s="6">
+        <f>Table1[[#This Row],[multiplier]]*Table1[[#This Row],[price]]</f>
+        <v>264.13200000000001</v>
+      </c>
+      <c r="K2" s="4">
+        <f>Table1[[#This Row],[etf_d]]/Table1[[#This Row],[etf_v]]</f>
+        <v>7.6767676767676776E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="5">
+        <v>23</v>
+      </c>
+      <c r="C3" s="4">
         <v>0.13</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>45691</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>3.83</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>52.38</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <f>Table1[[#This Row],[fwd_div]]/Table1[[#This Row],[price]]</f>
         <v>7.3119511263841155E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <v>13</v>
+      </c>
+      <c r="I3" s="6">
+        <f>Table1[[#This Row],[fwd_div]]*Table1[[#This Row],[multiplier]]</f>
+        <v>49.79</v>
+      </c>
+      <c r="J3" s="6">
+        <f>Table1[[#This Row],[multiplier]]*Table1[[#This Row],[price]]</f>
+        <v>680.94</v>
+      </c>
+      <c r="K3" s="4">
+        <f>Table1[[#This Row],[etf_d]]/Table1[[#This Row],[etf_v]]</f>
+        <v>7.3119511263841155E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="5">
+        <v>26</v>
+      </c>
+      <c r="C4" s="4">
         <v>0.1295</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>45691</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>1.3</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>20.48</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <f>Table1[[#This Row],[fwd_div]]/Table1[[#This Row],[price]]</f>
         <v>6.34765625E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>13</v>
+      </c>
+      <c r="I4" s="6">
+        <f>Table1[[#This Row],[fwd_div]]*Table1[[#This Row],[multiplier]]</f>
+        <v>16.900000000000002</v>
+      </c>
+      <c r="J4" s="6">
+        <f>Table1[[#This Row],[multiplier]]*Table1[[#This Row],[price]]</f>
+        <v>266.24</v>
+      </c>
+      <c r="K4" s="4">
+        <f>Table1[[#This Row],[etf_d]]/Table1[[#This Row],[etf_v]]</f>
+        <v>6.34765625E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="5">
+        <v>28</v>
+      </c>
+      <c r="C5" s="4">
         <v>0.12529999999999999</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>45691</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>3.5</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>40.28</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <f>Table1[[#This Row],[fwd_div]]/Table1[[#This Row],[price]]</f>
         <v>8.6891757696127114E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>13</v>
+      </c>
+      <c r="I5" s="6">
+        <f>Table1[[#This Row],[fwd_div]]*Table1[[#This Row],[multiplier]]</f>
+        <v>45.5</v>
+      </c>
+      <c r="J5" s="6">
+        <f>Table1[[#This Row],[multiplier]]*Table1[[#This Row],[price]]</f>
+        <v>523.64</v>
+      </c>
+      <c r="K5" s="4">
+        <f>Table1[[#This Row],[etf_d]]/Table1[[#This Row],[etf_v]]</f>
+        <v>8.6891757696127114E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="5">
+        <v>29</v>
+      </c>
+      <c r="C6" s="4">
         <v>0.1225</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>45691</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>2.14</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>32.65</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <f>Table1[[#This Row],[fwd_div]]/Table1[[#This Row],[price]]</f>
         <v>6.554364471669219E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>12</v>
+      </c>
+      <c r="I6" s="6">
+        <f>Table1[[#This Row],[fwd_div]]*Table1[[#This Row],[multiplier]]</f>
+        <v>25.68</v>
+      </c>
+      <c r="J6" s="6">
+        <f>Table1[[#This Row],[multiplier]]*Table1[[#This Row],[price]]</f>
+        <v>391.79999999999995</v>
+      </c>
+      <c r="K6" s="4">
+        <f>Table1[[#This Row],[etf_d]]/Table1[[#This Row],[etf_v]]</f>
+        <v>6.5543644716692204E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="5">
+        <v>30</v>
+      </c>
+      <c r="C7" s="4">
         <v>0.1133</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>45691</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>3.55</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>56.33</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <f>Table1[[#This Row],[fwd_div]]/Table1[[#This Row],[price]]</f>
         <v>6.3021480560979934E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>11</v>
+      </c>
+      <c r="I7" s="6">
+        <f>Table1[[#This Row],[fwd_div]]*Table1[[#This Row],[multiplier]]</f>
+        <v>39.049999999999997</v>
+      </c>
+      <c r="J7" s="6">
+        <f>Table1[[#This Row],[multiplier]]*Table1[[#This Row],[price]]</f>
+        <v>619.63</v>
+      </c>
+      <c r="K7" s="4">
+        <f>Table1[[#This Row],[etf_d]]/Table1[[#This Row],[etf_v]]</f>
+        <v>6.3021480560979934E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="5">
+        <v>31</v>
+      </c>
+      <c r="C8" s="4">
         <v>7.8399999999999997E-2</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>45691</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>2.8</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>40.51</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <f>Table1[[#This Row],[fwd_div]]/Table1[[#This Row],[price]]</f>
         <v>6.9118736114539614E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>8</v>
+      </c>
+      <c r="I8" s="6">
+        <f>Table1[[#This Row],[fwd_div]]*Table1[[#This Row],[multiplier]]</f>
+        <v>22.4</v>
+      </c>
+      <c r="J8" s="6">
+        <f>Table1[[#This Row],[multiplier]]*Table1[[#This Row],[price]]</f>
+        <v>324.08</v>
+      </c>
+      <c r="K8" s="4">
+        <f>Table1[[#This Row],[etf_d]]/Table1[[#This Row],[etf_v]]</f>
+        <v>6.9118736114539614E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="5">
+        <v>32</v>
+      </c>
+      <c r="C9" s="4">
         <v>4.6300000000000001E-2</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>45691</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>3.25</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>61.36</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <f>Table1[[#This Row],[fwd_div]]/Table1[[#This Row],[price]]</f>
         <v>5.2966101694915252E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9" s="6">
+        <f>Table1[[#This Row],[fwd_div]]*Table1[[#This Row],[multiplier]]</f>
+        <v>16.25</v>
+      </c>
+      <c r="J9" s="6">
+        <f>Table1[[#This Row],[multiplier]]*Table1[[#This Row],[price]]</f>
+        <v>306.8</v>
+      </c>
+      <c r="K9" s="4">
+        <f>Table1[[#This Row],[etf_d]]/Table1[[#This Row],[etf_v]]</f>
+        <v>5.2966101694915252E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="5">
+        <v>25</v>
+      </c>
+      <c r="C10" s="4">
         <v>2.6200000000000001E-2</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>45691</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>2.96</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>54.18</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <f>Table1[[#This Row],[fwd_div]]/Table1[[#This Row],[price]]</f>
         <v>5.4632705795496492E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10" s="6">
+        <f>Table1[[#This Row],[fwd_div]]*Table1[[#This Row],[multiplier]]</f>
+        <v>8.879999999999999</v>
+      </c>
+      <c r="J10" s="6">
+        <f>Table1[[#This Row],[multiplier]]*Table1[[#This Row],[price]]</f>
+        <v>162.54</v>
+      </c>
+      <c r="K10" s="4">
+        <f>Table1[[#This Row],[etf_d]]/Table1[[#This Row],[etf_v]]</f>
+        <v>5.4632705795496492E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="5">
+        <v>24</v>
+      </c>
+      <c r="C11" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>45691</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>1.3</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>21.13</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <f>Table1[[#This Row],[fwd_div]]/Table1[[#This Row],[price]]</f>
         <v>6.152389966871747E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11" s="6">
+        <f>Table1[[#This Row],[fwd_div]]*Table1[[#This Row],[multiplier]]</f>
+        <v>3.9000000000000004</v>
+      </c>
+      <c r="J11" s="6">
+        <f>Table1[[#This Row],[multiplier]]*Table1[[#This Row],[price]]</f>
+        <v>63.39</v>
+      </c>
+      <c r="K11" s="4">
+        <f>Table1[[#This Row],[etf_d]]/Table1[[#This Row],[etf_v]]</f>
+        <v>6.152389966871747E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="5">
+        <v>20</v>
+      </c>
+      <c r="C12" s="4">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>45691</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>0.66</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>10.52</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <f>Table1[[#This Row],[fwd_div]]/Table1[[#This Row],[price]]</f>
         <v>6.273764258555134E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12" s="6">
+        <f>Table1[[#This Row],[fwd_div]]*Table1[[#This Row],[multiplier]]</f>
+        <v>1.32</v>
+      </c>
+      <c r="J12" s="6">
+        <f>Table1[[#This Row],[multiplier]]*Table1[[#This Row],[price]]</f>
+        <v>21.04</v>
+      </c>
+      <c r="K12" s="4">
+        <f>Table1[[#This Row],[etf_d]]/Table1[[#This Row],[etf_v]]</f>
+        <v>6.273764258555134E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>1.3899999999999999E-2</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>45691</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>4.42</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <v>44.33</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <f>Table1[[#This Row],[fwd_div]]/Table1[[#This Row],[price]]</f>
         <v>9.9706744868035199E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C14" s="5"/>
-      <c r="E14" s="6">
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13" s="6">
+        <f>Table1[[#This Row],[fwd_div]]*Table1[[#This Row],[multiplier]]</f>
+        <v>4.42</v>
+      </c>
+      <c r="J13" s="6">
+        <f>Table1[[#This Row],[multiplier]]*Table1[[#This Row],[price]]</f>
+        <v>44.33</v>
+      </c>
+      <c r="K13" s="4">
+        <f>Table1[[#This Row],[etf_d]]/Table1[[#This Row],[etf_v]]</f>
+        <v>9.9706744868035199E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C14" s="4">
+        <f>SUBTOTAL(109,Table1[weight])</f>
+        <v>0.9648000000000001</v>
+      </c>
+      <c r="E14" s="5">
         <f>SUBTOTAL(109,Table1[fwd_div])</f>
         <v>31.230000000000004</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <f>SUBTOTAL(109,Table1[price])</f>
         <v>453.95</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <f>Table1[[#Totals],[fwd_div]]/Table1[[#Totals],[price]]</f>
         <v>6.8796122921026562E-2</v>
+      </c>
+      <c r="H14">
+        <f>SUBTOTAL(109,Table1[multiplier])</f>
+        <v>97.34</v>
+      </c>
+      <c r="I14" s="7">
+        <f>SUBTOTAL(109,Table1[etf_d])</f>
+        <v>254.36679999999998</v>
+      </c>
+      <c r="J14" s="7">
+        <f>SUBTOTAL(109,Table1[etf_v])</f>
+        <v>3668.5620000000004</v>
+      </c>
+      <c r="K14" s="4">
+        <f>Table1[[#Totals],[etf_d]]/Table1[[#Totals],[etf_v]]</f>
+        <v>6.9336922750658142E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>